<commit_message>
Con eventEmitter a medias
</commit_message>
<xml_diff>
--- a/Documentacion/API Results.xlsx
+++ b/Documentacion/API Results.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16340" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16340" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="characterized_products" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -80,9 +81,6 @@
     <t>showed</t>
   </si>
   <si>
-    <t>Selections</t>
-  </si>
-  <si>
     <t>ResultsComponent</t>
   </si>
   <si>
@@ -189,6 +187,50 @@
     </r>
   </si>
   <si>
+    <t>products_results: ProductResults[]</t>
+  </si>
+  <si>
+    <t>products: any[]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>Descripcion</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t xml:space="preserve">  Lo unico que hace es cambiar el formato de los registros del array products.   Cuando lo crea le pone showed='true' a todos los registros.  Es el array que va a dicatminar cuales productos se muestran en el cuerpo de la pagina dependiendo de los filtos. Hay que ver si se puede hacer mas directo con un pipe o map.</t>
+    </r>
+  </si>
+  <si>
+    <t>characterized_products: CharacterizedProducts[]   -   characterized_products_sorted</t>
+  </si>
+  <si>
+    <t>product_attributes: AttributesValues[]</t>
+  </si>
+  <si>
+    <t>Johny walker</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -224,17 +266,45 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">El array characterized_products recibe los datos crudos de la </t>
-    </r>
+      <t xml:space="preserve">A partir del array 'characterized_products' quita duplicados y deja combinaciones unicas de type_id y options_id </t>
+    </r>
+  </si>
+  <si>
+    <t>selected attribures</t>
+  </si>
+  <si>
+    <t>breadcrub</t>
+  </si>
+  <si>
+    <t>product_attributes1: AttributesValues[]</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
+        <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>API</t>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>Descripcion</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
     </r>
     <r>
       <rPr>
@@ -244,17 +314,39 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> del backend </t>
-    </r>
+      <t>A partir del array 'product_attributes' quiebra por type_id la informacion en 4 arrays, uno por type_id (restriccion arbitraria temporal)</t>
+    </r>
+  </si>
+  <si>
+    <t>product_attributes2: AttributesValues[]</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
+        <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'category_last_product_children_characterized'</t>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>Descripcion</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
     </r>
     <r>
       <rPr>
@@ -264,80 +356,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, despues se ordenan por type_id y options_id para tener todos los atributos filtrables y se guardan en el array characterized_products_sorted. Igual sospecho que characterized_products tambien queda ordenado.</t>
-    </r>
-  </si>
-  <si>
-    <t>products_results: ProductResults[]</t>
-  </si>
-  <si>
-    <t>products: any[]</t>
-  </si>
-  <si>
+      <t xml:space="preserve">El array characterized_products recibe los datos crudos de la </t>
+    </r>
     <r>
       <rPr>
         <b/>
-        <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri (Cuerpo)"/>
-      </rPr>
-      <t>Descripcion</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Cuerpo)"/>
-      </rPr>
-      <t>:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Cuerpo)"/>
-      </rPr>
-      <t xml:space="preserve">  Lo unico que hace es cambiar el formato de los registros del array products.   Cuando lo crea le pone showed='true' a todos los registros.  Es el array que va a dicatminar cuales productos se muestran en el cuerpo de la pagina dependiendo de los filtos. Hay que ver si se puede hacer mas directo con un pipe o map.</t>
-    </r>
-  </si>
-  <si>
-    <t>characterized_products: CharacterizedProducts[]   -   characterized_products_sorted</t>
-  </si>
-  <si>
-    <t>product_attributes: AttributesValues[]</t>
-  </si>
-  <si>
-    <t>Johny walker</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Cuerpo)"/>
-      </rPr>
-      <t>Descripcion</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Cuerpo)"/>
-      </rPr>
-      <t>:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Cuerpo)"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>API</t>
     </r>
     <r>
       <rPr>
@@ -347,45 +376,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">A partir del array 'characterized_products' quita duplicados y deja combinaciones unicas de type_id y options_id </t>
-    </r>
-  </si>
-  <si>
-    <t>selected attribures</t>
-  </si>
-  <si>
-    <t>breadcrub</t>
-  </si>
-  <si>
-    <t>product_attributes1: AttributesValues[]</t>
-  </si>
-  <si>
+      <t xml:space="preserve"> del backend </t>
+    </r>
     <r>
       <rPr>
         <b/>
-        <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri (Cuerpo)"/>
-      </rPr>
-      <t>Descripcion</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Cuerpo)"/>
-      </rPr>
-      <t>:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Cuerpo)"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'category_last_product_children_characterized'</t>
     </r>
     <r>
       <rPr>
@@ -395,11 +396,31 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>A partir del array 'product_attributes' quiebra por type_id la informacion en 4 arrays, uno por type_id (restriccion arbitraria temporal)</t>
-    </r>
-  </si>
-  <si>
-    <t>product_attributes2: AttributesValues[]</t>
+      <t xml:space="preserve"> a partir de la categoria/subcategoria seleccionada,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>despues se ordenan por type_id y options_id para tener todos los atributos filtrables y se guardan en el array characterized_products_sorted. Igual sospecho que characterized_products tambien queda ordenado.</t>
+    </r>
+  </si>
+  <si>
+    <t>Selected Atributes</t>
   </si>
 </sst>
 </file>
@@ -1458,10 +1479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:O83"/>
+  <dimension ref="B2:N83"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A48" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="J59" sqref="J59"/>
+    <sheetView showGridLines="0" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="G41" sqref="G38:G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1480,7 +1501,7 @@
   <sheetData>
     <row r="2" spans="2:13" ht="19" x14ac:dyDescent="0.25">
       <c r="B2" s="44" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="44"/>
       <c r="D2" s="44"/>
@@ -1515,7 +1536,7 @@
     <row r="5" spans="2:13" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="24"/>
       <c r="C5" s="16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
@@ -1530,7 +1551,7 @@
     <row r="6" spans="2:13" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="24"/>
       <c r="C6" s="41" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="42"/>
       <c r="E6" s="42"/>
@@ -1548,31 +1569,31 @@
         <v>0</v>
       </c>
       <c r="D7" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="37" t="s">
         <v>23</v>
-      </c>
-      <c r="E7" s="37" t="s">
-        <v>24</v>
       </c>
       <c r="F7" s="37" t="s">
         <v>3</v>
       </c>
       <c r="G7" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="37" t="s">
+      <c r="I7" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="37" t="s">
-        <v>27</v>
-      </c>
       <c r="J7" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="37" t="s">
+      <c r="L7" s="38" t="s">
         <v>21</v>
-      </c>
-      <c r="L7" s="38" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.2">
@@ -1666,7 +1687,7 @@
     <row r="17" spans="2:12" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="24"/>
       <c r="E17" s="16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
@@ -1677,7 +1698,7 @@
     <row r="18" spans="2:12" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="24"/>
       <c r="E18" s="45" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F18" s="46"/>
       <c r="G18" s="46"/>
@@ -1694,13 +1715,13 @@
         <v>3</v>
       </c>
       <c r="G19" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="H19" s="37" t="s">
+      <c r="I19" s="37" t="s">
         <v>24</v>
-      </c>
-      <c r="I19" s="37" t="s">
-        <v>25</v>
       </c>
       <c r="J19" s="38" t="s">
         <v>17</v>
@@ -1791,7 +1812,7 @@
     <row r="30" spans="2:12" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="24"/>
       <c r="C30" s="16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D30" s="17"/>
       <c r="E30" s="17"/>
@@ -1806,7 +1827,7 @@
     <row r="31" spans="2:12" ht="80" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" s="24"/>
       <c r="C31" s="48" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="D31" s="49"/>
       <c r="E31" s="49"/>
@@ -1841,7 +1862,7 @@
       <c r="I32" s="24"/>
       <c r="J32" s="24"/>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B33" s="24"/>
       <c r="C33" s="12">
         <v>2</v>
@@ -1864,7 +1885,7 @@
       <c r="I33" s="24"/>
       <c r="J33" s="24"/>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B34" s="24"/>
       <c r="C34" s="12">
         <v>4</v>
@@ -1887,7 +1908,7 @@
       <c r="I34" s="24"/>
       <c r="J34" s="24"/>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B35" s="24"/>
       <c r="C35" s="12">
         <v>5</v>
@@ -1909,8 +1930,11 @@
       </c>
       <c r="I35" s="24"/>
       <c r="J35" s="24"/>
-    </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B36" s="24"/>
       <c r="C36" s="12">
         <v>6</v>
@@ -1932,8 +1956,14 @@
       </c>
       <c r="I36" s="24"/>
       <c r="J36" s="24"/>
-    </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M36" t="s">
+        <v>15</v>
+      </c>
+      <c r="N36" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B37" s="24"/>
       <c r="C37" s="12">
         <v>1</v>
@@ -1955,8 +1985,14 @@
       </c>
       <c r="I37" s="24"/>
       <c r="J37" s="24"/>
-    </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M37">
+        <v>1</v>
+      </c>
+      <c r="N37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B38" s="24"/>
       <c r="C38" s="12">
         <v>3</v>
@@ -1979,7 +2015,7 @@
       <c r="I38" s="24"/>
       <c r="J38" s="24"/>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B39" s="24"/>
       <c r="C39" s="12">
         <v>7</v>
@@ -2001,11 +2037,14 @@
       </c>
       <c r="I39" s="24"/>
       <c r="J39" s="24"/>
-      <c r="N39" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M39">
+        <v>2</v>
+      </c>
+      <c r="N39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B40" s="24"/>
       <c r="C40" s="12">
         <v>12</v>
@@ -2027,14 +2066,8 @@
       </c>
       <c r="I40" s="24"/>
       <c r="J40" s="24"/>
-      <c r="N40" t="s">
-        <v>15</v>
-      </c>
-      <c r="O40" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B41" s="24"/>
       <c r="C41" s="12">
         <v>13</v>
@@ -2057,7 +2090,7 @@
       <c r="I41" s="24"/>
       <c r="J41" s="24"/>
     </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B42" s="24"/>
       <c r="C42" s="12">
         <v>10</v>
@@ -2080,7 +2113,7 @@
       <c r="I42" s="24"/>
       <c r="J42" s="24"/>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B43" s="24"/>
       <c r="C43" s="12">
         <v>11</v>
@@ -2103,7 +2136,7 @@
       <c r="I43" s="24"/>
       <c r="J43" s="24"/>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B44" s="24"/>
       <c r="C44" s="12">
         <v>14</v>
@@ -2126,7 +2159,7 @@
       <c r="I44" s="24"/>
       <c r="J44" s="24"/>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B45" s="24"/>
       <c r="C45" s="12">
         <v>16</v>
@@ -2149,7 +2182,7 @@
       <c r="I45" s="24"/>
       <c r="J45" s="24"/>
     </row>
-    <row r="46" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B46" s="24"/>
       <c r="C46" s="15">
         <v>15</v>
@@ -2172,12 +2205,12 @@
       <c r="I46" s="24"/>
       <c r="J46" s="24"/>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B47" s="24"/>
       <c r="K47" s="24"/>
       <c r="L47" s="24"/>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B48" s="24"/>
       <c r="K48" s="24"/>
       <c r="L48" s="24"/>
@@ -2197,7 +2230,7 @@
     <row r="51" spans="2:12" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="24"/>
       <c r="D51" s="32" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E51" s="33"/>
       <c r="F51" s="33"/>
@@ -2209,7 +2242,7 @@
     <row r="52" spans="2:12" ht="47" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B52" s="24"/>
       <c r="D52" s="58" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E52" s="59"/>
       <c r="F52" s="59"/>
@@ -2218,7 +2251,7 @@
       <c r="I52" s="24"/>
       <c r="J52" s="24"/>
       <c r="K52" s="62" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="53" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2258,7 +2291,7 @@
       <c r="I54" s="24"/>
       <c r="J54" s="24"/>
       <c r="K54" s="62" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="55" spans="2:12" x14ac:dyDescent="0.2">
@@ -2357,7 +2390,7 @@
         <v>7</v>
       </c>
       <c r="G60" s="53" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K60" s="24"/>
       <c r="L60" s="24"/>
@@ -2411,14 +2444,14 @@
     <row r="66" spans="2:12" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B66" s="24"/>
       <c r="D66" s="16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
       <c r="G66" s="17"/>
       <c r="H66" s="1"/>
       <c r="I66" s="16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J66" s="17"/>
       <c r="K66" s="17"/>
@@ -2427,14 +2460,14 @@
     <row r="67" spans="2:12" ht="47" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B67" s="24"/>
       <c r="D67" s="58" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E67" s="59"/>
       <c r="F67" s="59"/>
       <c r="G67" s="60"/>
       <c r="H67" s="1"/>
       <c r="I67" s="48" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J67" s="49"/>
       <c r="K67" s="49"/>
@@ -2563,7 +2596,7 @@
         <v>7</v>
       </c>
       <c r="L72" s="53" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="73" spans="2:12" x14ac:dyDescent="0.2">
@@ -2659,4 +2692,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>